<commit_message>
Added logic to commit to aws DB
</commit_message>
<xml_diff>
--- a/src/inputs/testing.xlsx
+++ b/src/inputs/testing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydrive.merck.com/personal/delrussa_merck_com/Documents/desktop/New_Vpack/src/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mydrive.merck.com/personal/delrussa_merck_com/Documents/desktop/Optimization_API/src/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="419" documentId="13_ncr:1_{7DDDAFBD-F520-4FED-9065-11E8EC85FDD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79128747-6A37-4F7F-AF40-092A44D68060}"/>
+  <xr:revisionPtr revIDLastSave="423" documentId="13_ncr:1_{7DDDAFBD-F520-4FED-9065-11E8EC85FDD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C526432-D209-4C93-B953-A27C1BE20766}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LROP" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Approvals!$A$1:$O$574</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LROP!$A$1:$K$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LROP!$A$1:$L$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3023" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3024" uniqueCount="111">
   <si>
     <t>Region</t>
   </si>
@@ -372,6 +372,9 @@
   </si>
   <si>
     <t>Launch_Month</t>
+  </si>
+  <si>
+    <t>Material_Number</t>
   </si>
 </sst>
 </file>
@@ -879,28 +882,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>86</v>
       </c>
@@ -908,70 +912,76 @@
         <v>5</v>
       </c>
       <c r="C1" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="22" t="s">
-        <v>0</v>
-      </c>
       <c r="F1" s="22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="I1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="J1" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="K1" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="L1" s="22" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>88</v>
       </c>
       <c r="B2">
         <v>2030</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>1234567</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>107</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>94</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>93</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>18200</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>1.4</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
@@ -1123,8 +1133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{380131F6-D988-40DF-B6FA-A4D0DEA9E81C}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>